<commit_message>
Check-in new group changes
</commit_message>
<xml_diff>
--- a/app/config/tables/Tea_houses/forms/Tea_houses/Tea_houses.xlsx
+++ b/app/config/tables/Tea_houses/forms/Tea_houses/Tea_houses.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="26330"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="5660" yWindow="5300" windowWidth="24740" windowHeight="23840" tabRatio="500" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="survey" sheetId="1" r:id="rId1"/>
@@ -166,9 +166,6 @@
     <t>No</t>
   </si>
   <si>
-    <t>Owner</t>
-  </si>
-  <si>
     <t>Phone_Number</t>
   </si>
   <si>
@@ -293,6 +290,9 @@
   </si>
   <si>
     <t>instance_name</t>
+  </si>
+  <si>
+    <t>Store_Owner</t>
   </si>
 </sst>
 </file>
@@ -645,7 +645,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -655,8 +655,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D39" sqref="D39"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -698,10 +698,10 @@
       </c>
       <c r="D2" s="3"/>
       <c r="E2" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="F2" s="2" t="s">
         <v>86</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>87</v>
       </c>
       <c r="G2" s="2"/>
     </row>
@@ -787,7 +787,7 @@
         <v>8</v>
       </c>
       <c r="E10" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="F10" t="s">
         <v>27</v>
@@ -798,7 +798,7 @@
         <v>5</v>
       </c>
       <c r="E11" t="s">
-        <v>46</v>
+        <v>88</v>
       </c>
       <c r="F11" t="s">
         <v>30</v>
@@ -809,7 +809,7 @@
         <v>5</v>
       </c>
       <c r="E12" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F12" t="s">
         <v>31</v>
@@ -859,16 +859,16 @@
     </row>
     <row r="16" spans="1:7">
       <c r="C16" t="s">
+        <v>69</v>
+      </c>
+      <c r="D16" t="s">
+        <v>79</v>
+      </c>
+      <c r="E16" t="s">
         <v>70</v>
       </c>
-      <c r="D16" t="s">
-        <v>80</v>
-      </c>
-      <c r="E16" t="s">
+      <c r="F16" t="s">
         <v>71</v>
-      </c>
-      <c r="F16" t="s">
-        <v>72</v>
       </c>
     </row>
   </sheetData>
@@ -942,7 +942,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
@@ -967,7 +967,7 @@
         <v>35</v>
       </c>
       <c r="B2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="4" spans="1:3">
@@ -975,7 +975,7 @@
         <v>36</v>
       </c>
       <c r="C4" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="5" spans="1:3">
@@ -983,7 +983,7 @@
         <v>37</v>
       </c>
       <c r="B5" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="30">
@@ -996,10 +996,10 @@
     </row>
     <row r="7" spans="1:3">
       <c r="A7" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B7" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
   </sheetData>
@@ -1024,13 +1024,13 @@
   <sheetData>
     <row r="1" spans="1:5">
       <c r="A1" t="s">
+        <v>47</v>
+      </c>
+      <c r="B1" t="s">
         <v>48</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>49</v>
-      </c>
-      <c r="C1" t="s">
-        <v>50</v>
       </c>
       <c r="D1" t="s">
         <v>16</v>
@@ -1041,121 +1041,121 @@
     </row>
     <row r="2" spans="1:5">
       <c r="A2" t="s">
+        <v>50</v>
+      </c>
+      <c r="B2" t="s">
         <v>51</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
         <v>52</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E2" t="s">
         <v>53</v>
-      </c>
-      <c r="D2" t="s">
-        <v>5</v>
-      </c>
-      <c r="E2" t="s">
-        <v>54</v>
       </c>
     </row>
     <row r="3" spans="1:5">
       <c r="A3" t="s">
+        <v>50</v>
+      </c>
+      <c r="B3" t="s">
         <v>51</v>
       </c>
-      <c r="B3" t="s">
-        <v>52</v>
-      </c>
       <c r="C3" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D3" t="s">
         <v>5</v>
       </c>
       <c r="E3" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="4" spans="1:5">
       <c r="A4" t="s">
+        <v>50</v>
+      </c>
+      <c r="B4" t="s">
         <v>51</v>
       </c>
-      <c r="B4" t="s">
-        <v>52</v>
-      </c>
       <c r="C4" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D4" t="s">
         <v>5</v>
       </c>
       <c r="E4" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="5" spans="1:5">
       <c r="A5" t="s">
+        <v>50</v>
+      </c>
+      <c r="B5" t="s">
         <v>51</v>
       </c>
-      <c r="B5" t="s">
-        <v>52</v>
-      </c>
       <c r="C5" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D5" t="s">
         <v>5</v>
       </c>
       <c r="E5" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="6" spans="1:5">
       <c r="A6" t="s">
+        <v>59</v>
+      </c>
+      <c r="B6" t="s">
+        <v>51</v>
+      </c>
+      <c r="C6" t="s">
         <v>60</v>
       </c>
-      <c r="B6" t="s">
-        <v>52</v>
-      </c>
-      <c r="C6" t="s">
+      <c r="D6" t="s">
+        <v>5</v>
+      </c>
+      <c r="E6" t="s">
         <v>61</v>
-      </c>
-      <c r="D6" t="s">
-        <v>5</v>
-      </c>
-      <c r="E6" t="s">
-        <v>62</v>
       </c>
     </row>
     <row r="7" spans="1:5">
       <c r="A7" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B7" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C7" t="s">
+        <v>62</v>
+      </c>
+      <c r="D7" t="s">
+        <v>5</v>
+      </c>
+      <c r="E7" t="s">
         <v>63</v>
-      </c>
-      <c r="D7" t="s">
-        <v>5</v>
-      </c>
-      <c r="E7" t="s">
-        <v>64</v>
       </c>
     </row>
     <row r="8" spans="1:5">
       <c r="A8" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B8" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C8" t="s">
+        <v>64</v>
+      </c>
+      <c r="D8" t="s">
+        <v>5</v>
+      </c>
+      <c r="E8" t="s">
         <v>65</v>
-      </c>
-      <c r="D8" t="s">
-        <v>5</v>
-      </c>
-      <c r="E8" t="s">
-        <v>66</v>
       </c>
     </row>
   </sheetData>
@@ -1189,48 +1189,48 @@
   <sheetData>
     <row r="1" spans="1:7">
       <c r="A1" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="B1" s="5" t="s">
         <v>73</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="C1" s="6" t="s">
         <v>74</v>
       </c>
-      <c r="C1" s="6" t="s">
+      <c r="D1" s="6" t="s">
         <v>75</v>
       </c>
-      <c r="D1" s="6" t="s">
+      <c r="E1" s="6" t="s">
         <v>76</v>
       </c>
-      <c r="E1" s="6" t="s">
+      <c r="F1" s="6" t="s">
         <v>77</v>
       </c>
-      <c r="F1" s="6" t="s">
+      <c r="G1" s="6" t="s">
         <v>78</v>
-      </c>
-      <c r="G1" s="6" t="s">
-        <v>79</v>
       </c>
     </row>
     <row r="2" spans="1:7">
       <c r="A2" t="s">
+        <v>79</v>
+      </c>
+      <c r="B2" t="s">
         <v>80</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
         <v>81</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
+        <v>81</v>
+      </c>
+      <c r="E2" t="s">
         <v>82</v>
       </c>
-      <c r="D2" t="s">
-        <v>82</v>
-      </c>
-      <c r="E2" t="s">
+      <c r="F2" t="s">
         <v>83</v>
       </c>
-      <c r="F2" t="s">
+      <c r="G2" s="7" t="s">
         <v>84</v>
-      </c>
-      <c r="G2" s="7" t="s">
-        <v>85</v>
       </c>
     </row>
   </sheetData>

</xml_diff>